<commit_message>
updated feature for first release
</commit_message>
<xml_diff>
--- a/dcomtestcasegeneration/Source/dcom/bin/Debug/DB_Requirement/RequirementDB_template.xlsx
+++ b/dcomtestcasegeneration/Source/dcom/bin/Debug/DB_Requirement/RequirementDB_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BGSV_EDA2_Automation_Tool_LOCALREPO\dcomtestcasegeneration\DCOMTestcaseGenerationR1.1\Source\dcom\bin\Debug\DB_Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D91C43-66D6-4EC8-ABD9-7D029F725521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D80DD3-1E25-422D-9AFE-C9AC0B0D76AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25845" yWindow="15" windowWidth="24855" windowHeight="15315" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Common_settings" sheetId="2" r:id="rId1"/>
@@ -1282,8 +1282,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4131,8 +4131,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:R17"/>
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4793,7 +4793,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:R17"/>
     </sheetView>
   </sheetViews>
@@ -6703,7 +6703,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
@@ -8207,7 +8207,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Z111"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1:Z5"/>
     </sheetView>
   </sheetViews>
@@ -10033,7 +10033,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:V111"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>

</xml_diff>